<commit_message>
Updated Test Data file path.
</commit_message>
<xml_diff>
--- a/Test Data/LoginData.xlsx
+++ b/Test Data/LoginData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neela\OneDrive\Desktop\JatinSharmaSDETMasterClass\automation-assignment\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261446D6-3ACD-4066-A2DB-9524ACF3A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6FD9F41E-EB8F-4373-92FD-F68148B98D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -368,7 +364,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Revert "Updated Test Data file path."
This reverts commit 597e6036a3bc3944dc7029eac0e973fc0938aa8d.
</commit_message>
<xml_diff>
--- a/Test Data/LoginData.xlsx
+++ b/Test Data/LoginData.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6FD9F41E-EB8F-4373-92FD-F68148B98D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neela\OneDrive\Desktop\JatinSharmaSDETMasterClass\automation-assignment\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261446D6-3ACD-4066-A2DB-9524ACF3A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -364,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>